<commit_message>
chore: start with book duckett HTML/CSS
</commit_message>
<xml_diff>
--- a/Guide for specialist.xlsx
+++ b/Guide for specialist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashmelkov/Education/FEWD/FEWD.RoadMap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashmelkov/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1550DD80-CEDE-A048-866C-2913695F01F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D11E927-597A-294D-9E82-E516CE71B433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{529C6E6D-FFA3-C64E-A9C2-3EBF424229B3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" xr2:uid="{529C6E6D-FFA3-C64E-A9C2-3EBF424229B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>0.1 Computer Science (50h)</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>1. Learn basics from a book</t>
-  </si>
-  <si>
-    <t>2. Go to websites: google, facebook, reddit,dribble</t>
   </si>
   <si>
     <t>3. curate all the micro-components that you like from these sites</t>
@@ -352,6 +349,21 @@
   </si>
   <si>
     <t xml:space="preserve">watch harvard short lection </t>
+  </si>
+  <si>
+    <t>Date/Deadline</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>2. Go to websites: google, facebook, reddit,dribble, cloudGuru</t>
+  </si>
+  <si>
+    <t>T - Theory</t>
+  </si>
+  <si>
+    <t>P - Practice</t>
   </si>
 </sst>
 </file>
@@ -367,7 +379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,6 +440,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF40FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -441,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -475,17 +493,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -498,12 +516,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF40FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -812,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDA43FD-2EDA-934B-A294-A3A2C5B3FDE9}">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,44 +865,48 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" customWidth="1"/>
     <col min="9" max="9" width="30.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="31.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" style="6" customWidth="1"/>
+    <col min="12" max="13" width="38" customWidth="1"/>
+    <col min="14" max="14" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -874,32 +914,38 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="8">
-        <f>1000-(SUM(J3:J996))</f>
+        <v>60</v>
+      </c>
+      <c r="K2" s="8">
+        <f>1000-(SUM(K3:K996))</f>
         <v>962</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -907,32 +953,36 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="3">
-        <v>3</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -942,124 +992,144 @@
       <c r="C4" s="2"/>
       <c r="D4" s="18"/>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="11">
+        <v>62</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K4" s="24">
         <v>1</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="18"/>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="13">
+        <v>63</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K5" s="24">
         <v>1</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="M5" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="11">
+        <v>64</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K6" s="24">
         <v>2</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="L6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" s="13">
+        <v>65</v>
+      </c>
+      <c r="J7" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K7" s="24">
         <v>1</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M7" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="19"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="13">
+      <c r="J8" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K8" s="24">
         <v>3</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M8" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="19"/>
       <c r="E9" s="2"/>
-      <c r="J9" s="13">
+      <c r="J9" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K9" s="24">
         <v>1</v>
       </c>
-      <c r="K9" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M9" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1067,256 +1137,304 @@
       <c r="C10" s="2"/>
       <c r="D10" s="19"/>
       <c r="E10" s="2"/>
-      <c r="J10" s="13">
+      <c r="J10" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K10" s="24">
         <v>3</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M10" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="19"/>
       <c r="E11" s="2"/>
-      <c r="J11" s="11">
+      <c r="J11" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K11" s="24">
         <v>2</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="17"/>
       <c r="C12" s="2"/>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="J12" s="13">
+      <c r="J12" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K12" s="24">
         <v>3</v>
       </c>
-      <c r="K12" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M12" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="17"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="J13" s="13">
+      <c r="J13" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K13" s="24">
         <v>3</v>
       </c>
-      <c r="K13" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M13" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="17"/>
       <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2"/>
       <c r="J14" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K14" s="24">
         <v>1.5</v>
       </c>
-      <c r="K14" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="26"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="17"/>
       <c r="C15" s="2"/>
       <c r="D15" s="20"/>
       <c r="E15" s="2"/>
-      <c r="J15" s="13">
+      <c r="J15" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K15" s="24">
         <v>2</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="17"/>
       <c r="C16" s="2"/>
       <c r="D16" s="20"/>
       <c r="E16" s="2"/>
-      <c r="J16" s="11">
+      <c r="J16" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K16" s="24">
         <v>1.5</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="20"/>
       <c r="E17" s="2"/>
-      <c r="J17" s="11">
+      <c r="J17" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K17" s="24">
         <v>1</v>
       </c>
-      <c r="K17" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="17"/>
       <c r="C18" s="2"/>
       <c r="D18" s="20"/>
       <c r="E18" s="2"/>
-      <c r="J18" s="13">
+      <c r="J18" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K18" s="24">
         <v>1</v>
       </c>
-      <c r="K18" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="17"/>
       <c r="C19" s="2"/>
       <c r="D19" s="20"/>
       <c r="E19" s="2"/>
-      <c r="J19" s="13">
+      <c r="J19" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K19" s="24">
         <v>5</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M19" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="17"/>
       <c r="C20" s="2"/>
       <c r="D20" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="J20" s="11">
+      <c r="J20" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K20" s="24">
         <v>2</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="17"/>
       <c r="C21" s="2"/>
       <c r="D21" s="21"/>
       <c r="E21" s="2"/>
-      <c r="J21" s="11">
+      <c r="J21" s="15">
+        <v>2020</v>
+      </c>
+      <c r="K21" s="24">
         <v>1</v>
       </c>
-      <c r="K21" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="17"/>
       <c r="C22" s="2"/>
       <c r="D22" s="21"/>
       <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J22" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="21"/>
       <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="J23" s="22">
+        <v>44468</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="17"/>
       <c r="C24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="17"/>
       <c r="C25" s="2"/>
       <c r="D25" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="17"/>
       <c r="C26" s="2"/>
       <c r="D26" s="17"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="17"/>
       <c r="C27" s="2"/>
       <c r="D27" s="17"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="17"/>
       <c r="C28" s="2"/>
       <c r="D28" s="17"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="17"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="17"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="17"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="17"/>
@@ -1325,11 +1443,11 @@
     <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="2"/>
     </row>
@@ -1443,7 +1561,7 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="2"/>
     </row>
@@ -1452,7 +1570,7 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50" s="2"/>
     </row>
@@ -1461,7 +1579,7 @@
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E51" s="2"/>
     </row>
@@ -1470,7 +1588,7 @@
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E52" s="2"/>
     </row>
@@ -1514,7 +1632,7 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" s="2"/>
     </row>
@@ -1523,7 +1641,7 @@
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E59" s="2"/>
     </row>
@@ -1562,102 +1680,103 @@
       <c r="D64" s="17"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="17"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="17"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="17"/>
       <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J69" s="16"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="17"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="17"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="17"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="17"/>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="17"/>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="17"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="17"/>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="17"/>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1666,6 +1785,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D68:D78"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="D33:D48"/>
+    <mergeCell ref="D52:D57"/>
+    <mergeCell ref="D59:D66"/>
     <mergeCell ref="B33:B44"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D7:D11"/>
@@ -1674,11 +1798,6 @@
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B23:B28"/>
-    <mergeCell ref="D68:D78"/>
-    <mergeCell ref="D25:D32"/>
-    <mergeCell ref="D33:D48"/>
-    <mergeCell ref="D52:D57"/>
-    <mergeCell ref="D59:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 1,5 for HTML CSS
</commit_message>
<xml_diff>
--- a/Guide for specialist.xlsx
+++ b/Guide for specialist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashmelkov/Education/SourceCode/FEWD/FEWD.RoadMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5817EE8-80DF-DC42-891F-D0C1F65FD5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66145C7A-A744-2842-AD2F-4812E0B5DAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" xr2:uid="{529C6E6D-FFA3-C64E-A9C2-3EBF424229B3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>0.1 Computer Science (50h)</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>Duckett HTML&amp;CSS - 3 - 4 chapter</t>
+  </si>
+  <si>
+    <t>Duckett HTML&amp;CSS - 5 chapter: images</t>
   </si>
 </sst>
 </file>
@@ -876,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDA43FD-2EDA-934B-A294-A3A2C5B3FDE9}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,7 +966,7 @@
       </c>
       <c r="K2" s="8">
         <f>1000-(SUM(K3:K996))</f>
-        <v>957.5</v>
+        <v>956</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>92</v>
@@ -1459,6 +1462,18 @@
       <c r="C27" s="2"/>
       <c r="D27" s="24"/>
       <c r="E27" s="2"/>
+      <c r="J27" s="17">
+        <v>44474</v>
+      </c>
+      <c r="K27" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>98</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -1848,6 +1863,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D68:D78"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="D33:D48"/>
+    <mergeCell ref="D52:D57"/>
+    <mergeCell ref="D59:D66"/>
     <mergeCell ref="B33:B44"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D7:D11"/>
@@ -1856,15 +1876,11 @@
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B23:B28"/>
-    <mergeCell ref="D68:D78"/>
-    <mergeCell ref="D25:D32"/>
-    <mergeCell ref="D33:D48"/>
-    <mergeCell ref="D52:D57"/>
-    <mergeCell ref="D59:D66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M25" r:id="rId1" xr:uid="{AFB02C4F-87B3-7A40-A334-08FBCB729A89}"/>
     <hyperlink ref="M26" r:id="rId2" xr:uid="{A7F0719D-256E-AA48-B705-F661124E9495}"/>
+    <hyperlink ref="M27" r:id="rId3" xr:uid="{416DB32B-378E-6E49-8D2D-1CBE65FBD4BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>